<commit_message>
update lab Tính năng Mail Merge
</commit_message>
<xml_diff>
--- a/word/lab8/dulieutronthu1/DSSV.xlsx
+++ b/word/lab8/dulieutronthu1/DSSV.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nentang\dao-tao\fpt\Tin-hoc\src\learning.nentang.vn-tin-hoc-can-ban\word\lab7\dulieutronthu1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nentang\dao-tao\fpt\Tin-hoc\src\learning.nentang.vn-tin-hoc-can-ban\word\lab8\dulieutronthu1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1999A1D1-CF9A-4ED3-8B33-3E7F3BFDA980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEE7C6C9-B11F-4843-AC9D-CC0A93488293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA189F8D-19D5-48AF-A821-D5C515CE9128}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +556,7 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.140625" customWidth="1"/>

</xml_diff>